<commit_message>
removed usless dirs; ISA table is 1stage_core doc complete
</commit_message>
<xml_diff>
--- a/scalar_cores/1stage_core/Docs/instructions.xlsb.xlsx
+++ b/scalar_cores/1stage_core/Docs/instructions.xlsb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NCSU_classes_files\spring20\633\Project\HMP\Heterogeneous-multicore\scalar_cores\5stage_core\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NCSU_classes_files\spring20\633\Project\HMP\Heterogeneous-multicore\scalar_cores\1stage_core\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE8AA97C-E4F4-4A94-A964-914A6EDE5490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF04D6A-606B-4BD9-95B8-A43D8C057664}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="369" firstSheet="1" activeTab="2" xr2:uid="{718E7806-298C-4F07-8385-55875B93F518}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="512" firstSheet="1" activeTab="2" xr2:uid="{718E7806-298C-4F07-8385-55875B93F518}"/>
   </bookViews>
   <sheets>
     <sheet name="Harris book ISA" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="mipstest" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="316">
   <si>
     <t>RTYPE</t>
   </si>
@@ -666,17 +665,351 @@
     <t>pc = pc + signex(imm); GPR[rd] = pc+4;</t>
   </si>
   <si>
-    <t>R type instn expansions</t>
-  </si>
-  <si>
-    <t>SLL, SRL, and SRA perform logical left, logical right, and arithmetic right shifts on the value in register rs1 by the shift amount held in the lower 5 bits of register rs2.</t>
+    <t>sub rd rs1 rs2</t>
+  </si>
+  <si>
+    <t>or rd rs1 rs2</t>
+  </si>
+  <si>
+    <t>slt rd rs1 rs2</t>
+  </si>
+  <si>
+    <t>GPR[rd] = GPR[rs1] - GPR[rs2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> and rd rs1 rs2</t>
+  </si>
+  <si>
+    <t>GPR[rd] = GPR[rs1] | GPR[rs2]</t>
+  </si>
+  <si>
+    <t>GPR[rd] = GPR[rs1] &amp; GPR[rs2]</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Arthmetic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Bitwise operations</t>
+    </r>
+  </si>
+  <si>
+    <t>[31:20]</t>
+  </si>
+  <si>
+    <t>SLTI</t>
+  </si>
+  <si>
+    <t>SLTIU</t>
+  </si>
+  <si>
+    <t>XORI</t>
+  </si>
+  <si>
+    <t>ORI</t>
+  </si>
+  <si>
+    <t>ANDI</t>
+  </si>
+  <si>
+    <t>SLLI</t>
+  </si>
+  <si>
+    <t>SRLI</t>
+  </si>
+  <si>
+    <t>SRAI</t>
+  </si>
+  <si>
+    <t>slti rd rs1 imm</t>
+  </si>
+  <si>
+    <t>sltiu rd rs1 imm</t>
+  </si>
+  <si>
+    <t>xori rd rs1 imm</t>
+  </si>
+  <si>
+    <t>ori rd rs1 imm</t>
+  </si>
+  <si>
+    <t>andi rd rs1 imm</t>
+  </si>
+  <si>
+    <t>slli rd rs1 imm</t>
+  </si>
+  <si>
+    <t>srli rd rs1 imm</t>
+  </si>
+  <si>
+    <t>srai rd rs1 imm</t>
+  </si>
+  <si>
+    <t>GPR[rd] = signed'(GPR[rs1]) &lt; signed'(signex[imm]) ? 1 : 0</t>
+  </si>
+  <si>
+    <t>GPR[rd] = GPR[rs1]  &lt; signex[imm] ? 1 : 0</t>
+  </si>
+  <si>
+    <t>GPR[rd] = GPR[rs1] ^ signex[imm]</t>
+  </si>
+  <si>
+    <t>GPR[rd] = GPR[rs1] | signex[imm]</t>
+  </si>
+  <si>
+    <t>GPR[rd] = GPR[rs1] &amp; signex[imm]</t>
+  </si>
+  <si>
+    <t>GPR[rd ] = GPR[rs1] &gt;&gt; GPR[rs2][4:0]</t>
+  </si>
+  <si>
+    <t>GPR[rd ] = GPR[rs1] &gt;&gt; signex[imm][4:0]</t>
+  </si>
+  <si>
+    <t>GPR[rd] = GPR[rs1] &lt;&lt; signex[imm][4:0]</t>
+  </si>
+  <si>
+    <t>GPR[rd] = {GPR[rs1], GPR[rs1]} &gt;&gt; signex[imm][4:0]</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>SLL</t>
+  </si>
+  <si>
+    <t>sll rd rs1 rs2</t>
+  </si>
+  <si>
+    <t>GPR[rd] = GPR[rs1] &lt;&lt; GPR[rs2][4:0]</t>
+  </si>
+  <si>
+    <t>SLTU</t>
+  </si>
+  <si>
+    <t>sltu rd rs1 rs2</t>
+  </si>
+  <si>
+    <t>GPR[rd] = (signed'(GPR[rs1]) &lt; signed'(GPR[rs2])) ? 1 : 0</t>
+  </si>
+  <si>
+    <t>XOR</t>
+  </si>
+  <si>
+    <t>xor rd rs1 rs2</t>
+  </si>
+  <si>
+    <t>GPR[rd] = GPR[rs1] ^ GPR[rs2]</t>
+  </si>
+  <si>
+    <t>GPR[rd] = {GPR[rs1], GPR[rs1]} &gt;&gt; GPR[rs2][4:0]</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>LH</t>
+  </si>
+  <si>
+    <t>LBU</t>
+  </si>
+  <si>
+    <t>LHW</t>
+  </si>
+  <si>
+    <t>lb rd imm(rs2)</t>
+  </si>
+  <si>
+    <t>lh rd imm(rs2)</t>
+  </si>
+  <si>
+    <t>lbu rd imm(rs2)</t>
+  </si>
+  <si>
+    <t>lhw rd imm(rs2)</t>
+  </si>
+  <si>
+    <t>addr = GPR[rs1]+signex[imm];  GPR[rd] = mem[addr[31:1]];</t>
+  </si>
+  <si>
+    <t>addr = GPR[rs1]+signex[imm];  GPR[rd] = mem[addr[31:2]];</t>
+  </si>
+  <si>
+    <t>addr = GPR[rs1]+signex[imm];  GPR[rd] = signex'mem[addr];</t>
+  </si>
+  <si>
+    <t>addr = GPR[rs1]+signex[imm];  GPR[rd] = signex'mem[addr[31:1]];</t>
+  </si>
+  <si>
+    <t>I-type - Immediate Arthmetic</t>
+  </si>
+  <si>
+    <t>I-type - Load Instns</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>addr = GPR[rs1]+signex[imm];  mem[addr[31:2]] = GPR[rs2][7:0];</t>
+  </si>
+  <si>
+    <t>addr = GPR[rs1]+signex[imm];  mem[addr[31:1]] = GPR[rs2][15:0];</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>BNE</t>
+  </si>
+  <si>
+    <t>BLT</t>
+  </si>
+  <si>
+    <t>BGE</t>
+  </si>
+  <si>
+    <t>BLTU</t>
+  </si>
+  <si>
+    <t>BGEU</t>
+  </si>
+  <si>
+    <t>bne rs1 rs2 imm</t>
+  </si>
+  <si>
+    <t>blt rs1 rs2 imm</t>
+  </si>
+  <si>
+    <t>bge rs1 rs2 imm</t>
+  </si>
+  <si>
+    <t>bltu rs1 rs2 imm</t>
+  </si>
+  <si>
+    <t>bgeu rs1 rs2 imm</t>
+  </si>
+  <si>
+    <t>target_pc = pc + signex(imm)</t>
+  </si>
+  <si>
+    <t>next_pc = (GPR[rs1] == GPR[rs2]) ? Target_pc : pcplus4</t>
+  </si>
+  <si>
+    <t>next_pc = (GPR[rs1] != GPR[rs2]) ? Target_pc : pcplus4</t>
+  </si>
+  <si>
+    <t>next_pc = (GPR[rs1] &lt; GPR[rs2]) ? Target_pc : pcplus4</t>
+  </si>
+  <si>
+    <t>next_pc = (GPR[rs1] &gt;= GPR[rs2]) ? Target_pc : pcplus4</t>
+  </si>
+  <si>
+    <t>next_pc = (unsigned'GPR[rs1] &lt; unsigned'GPR[rs2]) ? Target_pc : pcplus4</t>
+  </si>
+  <si>
+    <t>next_pc = (unsigned'GPR[rs1] &gt;= unsigned'GPR[rs2]) ? Target_pc : pcplus4</t>
+  </si>
+  <si>
+    <t>pc = target_pc; GPR[rd] = pc+4;</t>
+  </si>
+  <si>
+    <t>R-type - Arthmetic Reg to Reg</t>
+  </si>
+  <si>
+    <t>S-type - Store Instns</t>
+  </si>
+  <si>
+    <t>B-type - Branch Instns</t>
+  </si>
+  <si>
+    <t>J-type - JAL Unconditional jump and link instn</t>
+  </si>
+  <si>
+    <t>JALR</t>
+  </si>
+  <si>
+    <t>I-type - JALR Unconditional jump and link instn</t>
+  </si>
+  <si>
+    <t>1100111</t>
+  </si>
+  <si>
+    <t>jalr rd rs1 imm</t>
+  </si>
+  <si>
+    <t>pc = GPR[rs1] + signex(imm); GPR[rd] = pc+4;</t>
+  </si>
+  <si>
+    <t>LUI</t>
+  </si>
+  <si>
+    <t>AUIPC</t>
+  </si>
+  <si>
+    <t>0110111</t>
+  </si>
+  <si>
+    <t>0010111</t>
+  </si>
+  <si>
+    <t>lui rd imm</t>
+  </si>
+  <si>
+    <t>auipc rd imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GPR[rd] = utypeimm</t>
+  </si>
+  <si>
+    <t>utypeimm  = {instr[31:12], {12'b0}};</t>
+  </si>
+  <si>
+    <t>GPR[rd] = pc + utypeimm</t>
+  </si>
+  <si>
+    <t>Instn Count no</t>
+  </si>
+  <si>
+    <t>sb rs2 imm(rs1)</t>
+  </si>
+  <si>
+    <t>sh rs2 imm(rs1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -704,8 +1037,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -748,8 +1088,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -820,11 +1166,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -910,18 +1267,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -934,8 +1279,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1268,18 +1670,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
@@ -1527,18 +1929,18 @@
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
@@ -1565,20 +1967,20 @@
       <c r="I12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="37" t="s">
+      <c r="J12" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37" t="s">
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="37" t="s">
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="Q12" s="37"/>
+      <c r="Q12" s="43"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="14">
@@ -1605,20 +2007,20 @@
       <c r="I13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="36" t="s">
+      <c r="J13" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36" t="s">
+      <c r="K13" s="44"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="36" t="s">
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="Q13" s="36"/>
+      <c r="Q13" s="44"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
@@ -1627,14 +2029,14 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="38"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="47"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
@@ -1650,25 +2052,25 @@
       <c r="F15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37" t="s">
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37" t="s">
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37" t="s">
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="Q15" s="37"/>
+      <c r="Q15" s="43"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="14">
@@ -1686,25 +2088,25 @@
       <c r="F16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36" t="s">
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36" t="s">
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36" t="s">
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
+      <c r="P16" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="Q16" s="36"/>
+      <c r="Q16" s="44"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
@@ -1722,25 +2124,25 @@
       <c r="F17" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="G17" s="36" t="s">
+      <c r="G17" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36" t="s">
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36" t="s">
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="36" t="s">
+      <c r="N17" s="44"/>
+      <c r="O17" s="44"/>
+      <c r="P17" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="Q17" s="36"/>
+      <c r="Q17" s="44"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="14">
@@ -1758,25 +2160,25 @@
       <c r="F18" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G18" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36" t="s">
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36" t="s">
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36" t="s">
+      <c r="N18" s="44"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="Q18" s="36"/>
+      <c r="Q18" s="44"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="14">
@@ -1794,36 +2196,36 @@
       <c r="F19" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="36" t="s">
+      <c r="G19" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36" t="s">
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36" t="s">
+      <c r="K19" s="44"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36" t="s">
+      <c r="N19" s="44"/>
+      <c r="O19" s="44"/>
+      <c r="P19" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="Q19" s="36"/>
+      <c r="Q19" s="44"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="47"/>
+      <c r="P20" s="47"/>
+      <c r="Q20" s="47"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
@@ -1833,27 +2235,27 @@
       <c r="D21" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="37" t="s">
+      <c r="E21" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37" t="s">
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37" t="s">
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="N21" s="37"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="37" t="s">
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="Q21" s="37"/>
+      <c r="Q21" s="43"/>
     </row>
     <row r="22" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="14">
@@ -1865,32 +2267,32 @@
       <c r="D22" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="36" t="s">
+      <c r="E22" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36" t="s">
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36" t="s">
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="N22" s="36"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="41" t="s">
+      <c r="N22" s="44"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="Q22" s="41"/>
+      <c r="Q22" s="45"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="41"/>
+      <c r="P23" s="45"/>
+      <c r="Q23" s="45"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C24" s="23" t="s">
@@ -2037,6 +2439,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="C11:L11"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M17:O17"/>
     <mergeCell ref="E21:I21"/>
     <mergeCell ref="E22:I22"/>
     <mergeCell ref="P22:Q23"/>
@@ -2053,32 +2481,6 @@
     <mergeCell ref="P20:Q20"/>
     <mergeCell ref="P21:Q21"/>
     <mergeCell ref="J22:L22"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="C11:L11"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J15:L15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2090,7 +2492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8B24B8-6F90-4495-86A9-827C67D60825}">
   <dimension ref="B1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -2159,10 +2561,10 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="26" t="s">
         <v>151</v>
       </c>
@@ -2226,12 +2628,12 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="26" t="s">
         <v>153</v>
       </c>
@@ -2243,14 +2645,14 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43" t="s">
+      <c r="C9" s="50"/>
+      <c r="D9" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="E9" s="43"/>
+      <c r="E9" s="50"/>
       <c r="F9" s="32" t="s">
         <v>153</v>
       </c>
@@ -2440,10 +2842,10 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="51" t="s">
         <v>156</v>
       </c>
-      <c r="C21" s="44"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="6" t="s">
         <v>151</v>
       </c>
@@ -2461,10 +2863,10 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="C22" s="36"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="26" t="s">
         <v>151</v>
       </c>
@@ -2488,10 +2890,10 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="C23" s="36"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="26" t="s">
         <v>151</v>
       </c>
@@ -2634,14 +3036,14 @@
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43" t="s">
+      <c r="C31" s="50"/>
+      <c r="D31" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="E31" s="43"/>
+      <c r="E31" s="50"/>
       <c r="F31" s="32" t="s">
         <v>153</v>
       </c>
@@ -2653,14 +3055,14 @@
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36" t="s">
+      <c r="C32" s="44"/>
+      <c r="D32" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="E32" s="36"/>
+      <c r="E32" s="44"/>
       <c r="F32" s="26" t="s">
         <v>153</v>
       </c>
@@ -2679,17 +3081,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B21:C21"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2698,10 +3100,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A37AC45A-8A3E-4699-8562-56358E99A58E}">
-  <dimension ref="B1:J38"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2715,16 +3117,16 @@
     <col min="7" max="7" width="12" style="31" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="31"/>
     <col min="9" max="9" width="29.85546875" style="31" customWidth="1"/>
-    <col min="10" max="10" width="49.28515625" style="31" customWidth="1"/>
+    <col min="10" max="10" width="65.7109375" style="31" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F1" s="31" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="29" t="s">
         <v>170</v>
       </c>
@@ -2745,7 +3147,7 @@
       </c>
       <c r="H3" s="29"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
         <v>149</v>
       </c>
@@ -2768,11 +3170,11 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="36" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="30" t="s">
         <v>151</v>
       </c>
@@ -2789,7 +3191,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
         <v>158</v>
       </c>
@@ -2812,7 +3214,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="33" t="s">
         <v>191</v>
       </c>
@@ -2835,13 +3237,13 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="30" t="s">
         <v>153</v>
       </c>
@@ -2852,15 +3254,15 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="43" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43" t="s">
+      <c r="C9" s="50"/>
+      <c r="D9" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="E9" s="43"/>
+      <c r="E9" s="50"/>
       <c r="F9" s="33" t="s">
         <v>153</v>
       </c>
@@ -2871,12 +3273,24 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="62" t="s">
+        <v>313</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="62"/>
       <c r="B13" s="29" t="s">
         <v>170</v>
       </c>
@@ -2899,8 +3313,10 @@
       <c r="I13" s="29" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="37"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="62"/>
       <c r="B14" s="34" t="s">
         <v>149</v>
       </c>
@@ -2922,8 +3338,17 @@
       <c r="H14" s="34" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I14" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="J14" s="40" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="36">
+        <v>1</v>
+      </c>
       <c r="B15" s="3" t="s">
         <v>182</v>
       </c>
@@ -2945,18 +3370,21 @@
       <c r="H15" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="J15" s="31" t="s">
+      <c r="J15" s="52" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="36">
+        <v>2</v>
+      </c>
       <c r="B16" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="36" t="s">
         <v>150</v>
       </c>
       <c r="D16" s="30" t="s">
@@ -2974,366 +3402,1681 @@
       <c r="H16" s="30" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="J16" s="52" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="36">
+        <v>3</v>
+      </c>
       <c r="B17" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="36" t="s">
         <v>151</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F17" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="F17" s="36" t="s">
         <v>153</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="H17" s="30" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H17" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="I17" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="J17" s="36" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36">
+        <v>4</v>
+      </c>
       <c r="B18" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="36" t="s">
         <v>151</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="F18" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="F18" s="36" t="s">
         <v>153</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>180</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+      <c r="I18" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="J18" s="36" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="36">
+        <v>5</v>
+      </c>
       <c r="B19" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="36" t="s">
         <v>151</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="F19" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="F19" s="36" t="s">
         <v>153</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="H19" s="30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="45"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="45"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="34" t="s">
+      <c r="H19" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="I19" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="J19" s="36" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="36">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H20" s="36" t="s">
+        <v>254</v>
+      </c>
+      <c r="I20" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="J20" s="36" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="36">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H21" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="I21" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="J21" s="36" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="36">
+        <v>8</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H22" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="I22" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="J22" s="36" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="36">
+        <v>9</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H23" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="I23" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="J23" s="36" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="36">
+        <v>10</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="I24" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="J24" s="36" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="42"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="41"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="62" t="s">
+        <v>313</v>
+      </c>
+      <c r="B26" s="53" t="s">
+        <v>270</v>
+      </c>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+    </row>
+    <row r="27" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="62"/>
+      <c r="B27" s="54" t="s">
+        <v>218</v>
+      </c>
+      <c r="C27" s="55"/>
+      <c r="D27" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="G27" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="J27" s="37"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="62"/>
+      <c r="B28" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="C28" s="51"/>
+      <c r="D28" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="H28" s="34" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="44" t="s">
+      <c r="I28" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="J28" s="40"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="36">
+        <v>11</v>
+      </c>
+      <c r="B29" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" s="34" t="s">
+      <c r="C29" s="44"/>
+      <c r="D29" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="E29" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H29" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="36" t="s">
+        <v>199</v>
+      </c>
+      <c r="J29" s="36" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="36">
+        <v>12</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="44"/>
+      <c r="D30" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F30" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H30" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="I30" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="J30" s="36" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="36">
+        <v>13</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C31" s="44"/>
+      <c r="D31" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H31" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="I31" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="J31" s="36" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="36">
+        <v>14</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" s="44"/>
+      <c r="D32" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F32" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H32" s="36" t="s">
+        <v>221</v>
+      </c>
+      <c r="I32" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="J32" s="36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="36">
+        <v>15</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C33" s="44"/>
+      <c r="D33" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F33" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H33" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="I33" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="J33" s="36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="36">
+        <v>16</v>
+      </c>
+      <c r="B34" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="44"/>
+      <c r="D34" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F34" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H34" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="I34" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="J34" s="36" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="36">
+        <v>17</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="D35" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="F35" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H35" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="I35" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="J35" s="36" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="36">
+        <v>18</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="D36" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H36" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="I36" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="J36" s="36" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="36">
+        <v>19</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="D37" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F37" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H37" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="I37" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="J37" s="36" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="41"/>
+    </row>
+    <row r="39" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="62" t="s">
+        <v>313</v>
+      </c>
+      <c r="B39" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="53"/>
+    </row>
+    <row r="40" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="62"/>
+      <c r="B40" s="54" t="s">
+        <v>218</v>
+      </c>
+      <c r="C40" s="55"/>
+      <c r="D40" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="E40" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="F40" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="G40" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="J40" s="37" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="62"/>
+      <c r="B41" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" s="51"/>
+      <c r="D41" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="E41" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="F23" s="34" t="s">
+      <c r="F41" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="G23" s="34" t="s">
+      <c r="G41" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="H23" s="34" t="s">
+      <c r="H41" s="40" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="36" t="s">
+      <c r="I41" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="J41" s="40"/>
+    </row>
+    <row r="42" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="36">
+        <v>20</v>
+      </c>
+      <c r="B42" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="C42" s="44"/>
+      <c r="D42" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="F24" s="30" t="s">
+      <c r="F42" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H42" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="I42" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="J42" s="36" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="36">
+        <v>21</v>
+      </c>
+      <c r="B43" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C43" s="44"/>
+      <c r="D43" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H43" s="36" t="s">
+        <v>259</v>
+      </c>
+      <c r="I43" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="J43" s="36" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="36">
+        <v>22</v>
+      </c>
+      <c r="B44" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" s="44"/>
+      <c r="D44" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F44" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H44" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="I44" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="J44" s="36" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="36">
+        <v>23</v>
+      </c>
+      <c r="B45" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" s="44"/>
+      <c r="D45" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F45" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H45" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="I45" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="J45" s="36" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="36">
+        <v>24</v>
+      </c>
+      <c r="B46" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" s="44"/>
+      <c r="D46" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F46" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H46" s="36" t="s">
+        <v>261</v>
+      </c>
+      <c r="I46" s="36" t="s">
+        <v>265</v>
+      </c>
+      <c r="J46" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="42"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="41"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="62" t="s">
+        <v>313</v>
+      </c>
+      <c r="B48" s="53" t="s">
+        <v>296</v>
+      </c>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="53"/>
+      <c r="J48" s="53"/>
+    </row>
+    <row r="49" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="62"/>
+      <c r="B49" s="43" t="s">
+        <v>218</v>
+      </c>
+      <c r="C49" s="43"/>
+      <c r="D49" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="E49" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="F49" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="G49" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="J49" s="37" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="62"/>
+      <c r="B50" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="D50" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="E50" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="F50" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="G50" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="H50" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="I50" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="J50" s="40"/>
+    </row>
+    <row r="51" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="36">
+        <v>25</v>
+      </c>
+      <c r="B51" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C51" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D51" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F51" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H51" s="36" t="s">
+        <v>272</v>
+      </c>
+      <c r="I51" s="36" t="s">
+        <v>314</v>
+      </c>
+      <c r="J51" s="36" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="36">
+        <v>26</v>
+      </c>
+      <c r="B52" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C52" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D52" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="F52" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H52" s="36" t="s">
+        <v>273</v>
+      </c>
+      <c r="I52" s="36" t="s">
+        <v>315</v>
+      </c>
+      <c r="J52" s="36" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="36">
+        <v>27</v>
+      </c>
+      <c r="B53" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C53" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D53" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F53" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H53" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="I53" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="J53" s="36" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="41"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="41"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="41"/>
+    </row>
+    <row r="55" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="41"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="41"/>
+      <c r="E55" s="42"/>
+      <c r="F55" s="41"/>
+      <c r="G55" s="42"/>
+      <c r="H55" s="41"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="62" t="s">
+        <v>313</v>
+      </c>
+      <c r="B56" s="51" t="s">
+        <v>297</v>
+      </c>
+      <c r="C56" s="51"/>
+      <c r="D56" s="51"/>
+      <c r="E56" s="51"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="51"/>
+      <c r="H56" s="51"/>
+      <c r="I56" s="51"/>
+      <c r="J56" s="51"/>
+    </row>
+    <row r="57" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="62"/>
+      <c r="B57" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="C57" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="D57" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="E57" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="F57" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="G57" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="J57" s="37"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="62"/>
+      <c r="B58" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="C58" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="D58" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="E58" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="F58" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="G58" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="H58" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="I58" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="J58" s="39" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="36">
+        <v>28</v>
+      </c>
+      <c r="B59" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="C59" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="D59" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F59" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H59" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I59" s="36" t="s">
+        <v>205</v>
+      </c>
+      <c r="J59" s="36" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="36">
+        <v>29</v>
+      </c>
+      <c r="B60" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="C60" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D60" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="F60" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H60" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="I60" s="36" t="s">
+        <v>282</v>
+      </c>
+      <c r="J60" s="36" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="36">
+        <v>30</v>
+      </c>
+      <c r="B61" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="C61" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D61" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F61" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H61" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="I61" s="36" t="s">
+        <v>283</v>
+      </c>
+      <c r="J61" s="36" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="36">
+        <v>31</v>
+      </c>
+      <c r="B62" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="C62" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F62" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H62" s="36" t="s">
+        <v>279</v>
+      </c>
+      <c r="I62" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="J62" s="36" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="36">
+        <v>32</v>
+      </c>
+      <c r="B63" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D63" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F63" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H63" s="36" t="s">
+        <v>280</v>
+      </c>
+      <c r="I63" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="J63" s="36" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="36">
+        <v>33</v>
+      </c>
+      <c r="B64" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D64" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F64" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H64" s="36" t="s">
+        <v>281</v>
+      </c>
+      <c r="I64" s="36" t="s">
+        <v>286</v>
+      </c>
+      <c r="J64" s="36" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="41"/>
+      <c r="C65" s="41"/>
+      <c r="D65" s="41"/>
+      <c r="E65" s="42"/>
+      <c r="F65" s="41"/>
+      <c r="G65" s="42"/>
+      <c r="H65" s="41"/>
+    </row>
+    <row r="66" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="41"/>
+      <c r="C66" s="41"/>
+      <c r="D66" s="41"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="41"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="41"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="62" t="s">
+        <v>313</v>
+      </c>
+      <c r="B67" s="51" t="s">
+        <v>298</v>
+      </c>
+      <c r="C67" s="51"/>
+      <c r="D67" s="51"/>
+      <c r="E67" s="51"/>
+      <c r="F67" s="51"/>
+      <c r="G67" s="51"/>
+      <c r="H67" s="51"/>
+      <c r="I67" s="51"/>
+      <c r="J67" s="51"/>
+    </row>
+    <row r="68" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="62"/>
+      <c r="B68" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="C68" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="D68" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="E68" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="F68" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="G68" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="J68" s="37"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="62"/>
+      <c r="B69" s="57" t="s">
+        <v>172</v>
+      </c>
+      <c r="C69" s="57"/>
+      <c r="D69" s="57" t="s">
+        <v>173</v>
+      </c>
+      <c r="E69" s="57"/>
+      <c r="F69" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H24" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="I24" s="31" t="s">
-        <v>199</v>
-      </c>
-      <c r="J24" s="31" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="36" t="s">
+      <c r="G69" s="58" t="s">
+        <v>154</v>
+      </c>
+      <c r="H69" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="I69" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="J69" s="39" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="36">
+        <v>34</v>
+      </c>
+      <c r="B70" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="C70" s="44"/>
+      <c r="D70" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="E70" s="44"/>
+      <c r="F70" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H70" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="I70" s="36" t="s">
+        <v>207</v>
+      </c>
+      <c r="J70" s="36" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="62" t="s">
+        <v>313</v>
+      </c>
+      <c r="B72" s="53" t="s">
+        <v>300</v>
+      </c>
+      <c r="C72" s="53"/>
+      <c r="D72" s="53"/>
+      <c r="E72" s="53"/>
+      <c r="F72" s="53"/>
+      <c r="G72" s="53"/>
+      <c r="H72" s="53"/>
+      <c r="I72" s="53"/>
+      <c r="J72" s="53"/>
+    </row>
+    <row r="73" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="62"/>
+      <c r="B73" s="54" t="s">
+        <v>218</v>
+      </c>
+      <c r="C73" s="55"/>
+      <c r="D73" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="E73" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="F73" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="G73" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="H73" s="37"/>
+      <c r="I73" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="J73" s="37"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="62"/>
+      <c r="B74" s="60" t="s">
         <v>156</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H25" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="I25" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="J25" s="31" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="34" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="C27" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="D27" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="E27" s="34" t="s">
+      <c r="C74" s="61"/>
+      <c r="D74" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="E74" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="F27" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="G27" s="34" t="s">
+      <c r="F74" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="G74" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="H27" s="34" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="F28" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="H28" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="I28" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="J28" s="31" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="35" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="D30" s="33" t="s">
-        <v>151</v>
-      </c>
-      <c r="E30" s="33" t="s">
-        <v>152</v>
-      </c>
-      <c r="F30" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="G30" s="33" t="s">
+      <c r="H74" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="I74" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="J74" s="40"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="36">
+        <v>35</v>
+      </c>
+      <c r="B75" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="C75" s="44"/>
+      <c r="D75" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F75" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="H75" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="I75" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="J75" s="36" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="62" t="s">
+        <v>313</v>
+      </c>
+      <c r="B77" s="53" t="s">
+        <v>163</v>
+      </c>
+      <c r="C77" s="53"/>
+      <c r="D77" s="53"/>
+      <c r="E77" s="53"/>
+      <c r="F77" s="53"/>
+      <c r="G77" s="53"/>
+      <c r="H77" s="53"/>
+      <c r="I77" s="53"/>
+      <c r="J77" s="53"/>
+    </row>
+    <row r="78" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="62"/>
+      <c r="B78" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="C78" s="59"/>
+      <c r="D78" s="59"/>
+      <c r="E78" s="55"/>
+      <c r="F78" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="G78" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="H78" s="37"/>
+      <c r="I78" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="J78" s="37"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="62"/>
+      <c r="B79" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C79" s="51"/>
+      <c r="D79" s="51"/>
+      <c r="E79" s="51"/>
+      <c r="F79" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="G79" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="H30" s="33" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="D31" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>171</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="H31" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="I31" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="J31" s="31" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="35" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="43" t="s">
-        <v>172</v>
-      </c>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43" t="s">
-        <v>173</v>
-      </c>
-      <c r="E33" s="43"/>
-      <c r="F33" s="33" t="s">
+      <c r="H79" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="I79" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="J79" s="40" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="36">
+        <v>36</v>
+      </c>
+      <c r="B80" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="C80" s="44"/>
+      <c r="D80" s="44"/>
+      <c r="E80" s="44"/>
+      <c r="F80" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="G33" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="H33" s="33" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="36" t="s">
-        <v>172</v>
-      </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="30" t="s">
+      <c r="G80" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="H80" s="36" t="s">
+        <v>304</v>
+      </c>
+      <c r="I80" s="36" t="s">
+        <v>308</v>
+      </c>
+      <c r="J80" s="36" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="36">
+        <v>37</v>
+      </c>
+      <c r="B81" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="C81" s="44"/>
+      <c r="D81" s="44"/>
+      <c r="E81" s="44"/>
+      <c r="F81" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="H34" s="30" t="s">
-        <v>195</v>
-      </c>
-      <c r="I34" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="J34" s="31" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="31" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="47" t="s">
-        <v>210</v>
-      </c>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
+      <c r="G81" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="H81" s="36" t="s">
+        <v>305</v>
+      </c>
+      <c r="I81" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="J81" s="36" t="s">
+        <v>312</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B38:E38"/>
+  <mergeCells count="47">
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="B77:J77"/>
+    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B48:J48"/>
+    <mergeCell ref="B56:J56"/>
+    <mergeCell ref="B67:J67"/>
+    <mergeCell ref="B72:J72"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B39:J39"/>
+    <mergeCell ref="B49:C49"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added instn_type 3d associative array in debug_package of 1stage_core | hello world example changed - console address is 65536
</commit_message>
<xml_diff>
--- a/scalar_cores/1stage_core/Docs/instructions.xlsb.xlsx
+++ b/scalar_cores/1stage_core/Docs/instructions.xlsb.xlsx
@@ -668,7 +668,27 @@
     <t xml:space="preserve">lbu rd imm(rs2)</t>
   </si>
   <si>
-    <t xml:space="preserve">LHW</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">LH</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">U</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">lhw rd imm(rs2)</t>
@@ -1014,12 +1034,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[H]:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="0.00E+00"/>
+    <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1060,6 +1081,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1249,10 +1278,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1309,6 +1334,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1321,7 +1350,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1416,7 +1445,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="18.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.42"/>
@@ -1839,10 +1868,10 @@
       <c r="D16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G16" s="12" t="s">
@@ -1875,10 +1904,10 @@
       <c r="D17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="7" t="s">
         <v>49</v>
       </c>
       <c r="G17" s="12" t="s">
@@ -1911,10 +1940,10 @@
       <c r="D18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G18" s="12" t="s">
@@ -1947,10 +1976,10 @@
       <c r="D19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G19" s="12" t="s">
@@ -1989,7 +2018,7 @@
       <c r="C21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="16" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="11" t="s">
@@ -2036,28 +2065,28 @@
       </c>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
-      <c r="M22" s="18" t="s">
+      <c r="M22" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="19" t="s">
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="Q22" s="19"/>
+      <c r="Q22" s="18"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="14"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="22"/>
+      <c r="D24" s="20"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="21"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="14"/>
@@ -2067,8 +2096,8 @@
       <c r="D25" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="7" t="s">
@@ -2079,7 +2108,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="20" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="10" t="s">
@@ -2141,10 +2170,10 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="23"/>
+      <c r="D36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="n">
@@ -2158,7 +2187,7 @@
       <c r="C38" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="D38" s="24" t="s">
+      <c r="D38" s="23" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2174,7 +2203,7 @@
       <c r="C41" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="24" t="s">
+      <c r="D41" s="23" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2190,7 +2219,7 @@
       <c r="C44" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D44" s="24" t="s">
+      <c r="D44" s="23" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2262,17 +2291,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="15.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="13" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="13" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="13" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="13" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="13" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="13" width="29.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="13" width="49.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="13" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="13" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2369,25 +2398,25 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="25" t="s">
+      <c r="D7" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="24" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2409,21 +2438,21 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="24"/>
+      <c r="D9" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25" t="s">
+      <c r="E9" s="24"/>
+      <c r="F9" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2738,30 +2767,30 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="25" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="E28" s="25" t="s">
+      <c r="D28" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="F28" s="25" t="s">
+      <c r="F28" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="G28" s="25" t="s">
+      <c r="G28" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="H28" s="25" t="s">
+      <c r="H28" s="24" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2795,26 +2824,26 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="25" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25" t="s">
+      <c r="C31" s="24"/>
+      <c r="D31" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25" t="s">
+      <c r="E31" s="24"/>
+      <c r="F31" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="G31" s="25" t="s">
+      <c r="G31" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="H31" s="25" t="s">
+      <c r="H31" s="24" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2872,25 +2901,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L28" activeCellId="0" sqref="L28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N47" activeCellId="0" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="15.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="13" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="13" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="13" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="13" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="13" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="13" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="13" width="65.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="13" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="13" width="65.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="13" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2987,25 +3016,25 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="25" t="s">
+      <c r="D7" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="24" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3027,42 +3056,42 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="24"/>
+      <c r="D9" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25" t="s">
+      <c r="E9" s="24"/>
+      <c r="F9" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="27"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="11" t="s">
         <v>81</v>
       </c>
@@ -3088,7 +3117,7 @@
       <c r="J13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="6" t="s">
         <v>87</v>
       </c>
@@ -3113,7 +3142,7 @@
       <c r="I14" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="28" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3145,7 +3174,7 @@
       <c r="I15" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="J15" s="30" t="s">
+      <c r="J15" s="29" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3177,7 +3206,7 @@
       <c r="I16" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="J16" s="30" t="s">
+      <c r="J16" s="29" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3447,23 +3476,26 @@
       <c r="H25" s="15"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="M26" s="30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="27"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="11" t="s">
         <v>172</v>
       </c>
@@ -3487,7 +3519,7 @@
       <c r="J27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="27"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="6" t="s">
         <v>94</v>
       </c>
@@ -3798,23 +3830,23 @@
       <c r="H38" s="15"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="28"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="27"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="11" t="s">
         <v>172</v>
       </c>
@@ -3840,7 +3872,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="27"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="6" t="s">
         <v>94</v>
       </c>
@@ -3985,7 +4017,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="n">
         <v>24</v>
       </c>
@@ -4027,23 +4059,23 @@
       <c r="J47" s="15"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="27" t="s">
+      <c r="A48" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="B48" s="28" t="s">
+      <c r="B48" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="28"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="28"/>
-      <c r="I48" s="28"/>
-      <c r="J48" s="28"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="27"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="27"/>
+      <c r="A49" s="26"/>
       <c r="B49" s="11" t="s">
         <v>172</v>
       </c>
@@ -4069,7 +4101,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="27"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="6" t="s">
         <v>96</v>
       </c>
@@ -4211,7 +4243,7 @@
       <c r="H55" s="15"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="27" t="s">
+      <c r="A56" s="26" t="s">
         <v>140</v>
       </c>
       <c r="B56" s="6" t="s">
@@ -4227,7 +4259,7 @@
       <c r="J56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="27"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="11" t="s">
         <v>81</v>
       </c>
@@ -4253,32 +4285,32 @@
       <c r="J57" s="11"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="27"/>
-      <c r="B58" s="25" t="s">
+      <c r="A58" s="26"/>
+      <c r="B58" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="C58" s="25" t="s">
+      <c r="C58" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D58" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="E58" s="25" t="s">
+      <c r="D58" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E58" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="F58" s="25" t="s">
+      <c r="F58" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="G58" s="25" t="s">
+      <c r="G58" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="H58" s="25" t="s">
+      <c r="H58" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="I58" s="25" t="s">
+      <c r="I58" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="J58" s="25" t="s">
+      <c r="J58" s="24" t="s">
         <v>220</v>
       </c>
     </row>
@@ -4493,7 +4525,7 @@
       <c r="H66" s="15"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="27" t="s">
+      <c r="A67" s="26" t="s">
         <v>140</v>
       </c>
       <c r="B67" s="6" t="s">
@@ -4509,7 +4541,7 @@
       <c r="J67" s="6"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="27"/>
+      <c r="A68" s="26"/>
       <c r="B68" s="11" t="s">
         <v>81</v>
       </c>
@@ -4535,7 +4567,7 @@
       <c r="J68" s="11"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="27"/>
+      <c r="A69" s="26"/>
       <c r="B69" s="31" t="s">
         <v>104</v>
       </c>
@@ -4553,10 +4585,10 @@
       <c r="H69" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="I69" s="25" t="s">
+      <c r="I69" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="J69" s="25" t="s">
+      <c r="J69" s="24" t="s">
         <v>220</v>
       </c>
     </row>
@@ -4589,23 +4621,23 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="27" t="s">
+      <c r="A72" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="B72" s="28" t="s">
+      <c r="B72" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
-      <c r="E72" s="28"/>
-      <c r="F72" s="28"/>
-      <c r="G72" s="28"/>
-      <c r="H72" s="28"/>
-      <c r="I72" s="28"/>
-      <c r="J72" s="28"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="27"/>
+      <c r="H72" s="27"/>
+      <c r="I72" s="27"/>
+      <c r="J72" s="27"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="27"/>
+      <c r="A73" s="26"/>
       <c r="B73" s="11" t="s">
         <v>172</v>
       </c>
@@ -4629,7 +4661,7 @@
       <c r="J73" s="11"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="27"/>
+      <c r="A74" s="26"/>
       <c r="B74" s="6" t="s">
         <v>94</v>
       </c>
@@ -4685,23 +4717,23 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="27" t="s">
+      <c r="A77" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="B77" s="28" t="s">
+      <c r="B77" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="C77" s="28"/>
-      <c r="D77" s="28"/>
-      <c r="E77" s="28"/>
-      <c r="F77" s="28"/>
-      <c r="G77" s="28"/>
-      <c r="H77" s="28"/>
-      <c r="I77" s="28"/>
-      <c r="J77" s="28"/>
+      <c r="C77" s="27"/>
+      <c r="D77" s="27"/>
+      <c r="E77" s="27"/>
+      <c r="F77" s="27"/>
+      <c r="G77" s="27"/>
+      <c r="H77" s="27"/>
+      <c r="I77" s="27"/>
+      <c r="J77" s="27"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="27"/>
+      <c r="A78" s="26"/>
       <c r="B78" s="11" t="s">
         <v>102</v>
       </c>
@@ -4721,7 +4753,7 @@
       <c r="J78" s="11"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="27"/>
+      <c r="A79" s="26"/>
       <c r="B79" s="6" t="s">
         <v>102</v>
       </c>
@@ -4893,82 +4925,82 @@
       <c r="E4" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="F4" s="23" t="n">
+      <c r="F4" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="23" t="n">
+      <c r="G4" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="H4" s="23" t="n">
+      <c r="H4" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="I4" s="23" t="n">
+      <c r="I4" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="J4" s="23" t="n">
+      <c r="J4" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="K4" s="23" t="n">
+      <c r="K4" s="22" t="n">
         <v>5</v>
       </c>
-      <c r="L4" s="23" t="n">
+      <c r="L4" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="M4" s="23" t="n">
+      <c r="M4" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="N4" s="23" t="n">
+      <c r="N4" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="O4" s="23" t="n">
+      <c r="O4" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="P4" s="23" t="n">
+      <c r="P4" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="Q4" s="23" t="n">
+      <c r="Q4" s="22" t="n">
         <v>11</v>
       </c>
-      <c r="R4" s="23" t="n">
+      <c r="R4" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="S4" s="23" t="n">
+      <c r="S4" s="22" t="n">
         <v>13</v>
       </c>
-      <c r="T4" s="23" t="n">
+      <c r="T4" s="22" t="n">
         <v>14</v>
       </c>
-      <c r="U4" s="23" t="n">
+      <c r="U4" s="22" t="n">
         <v>15</v>
       </c>
-      <c r="V4" s="23" t="n">
+      <c r="V4" s="22" t="n">
         <v>16</v>
       </c>
-      <c r="W4" s="23" t="n">
+      <c r="W4" s="22" t="n">
         <v>17</v>
       </c>
-      <c r="X4" s="23" t="n">
+      <c r="X4" s="22" t="n">
         <v>18</v>
       </c>
-      <c r="Y4" s="23" t="n">
+      <c r="Y4" s="22" t="n">
         <v>19</v>
       </c>
-      <c r="Z4" s="23" t="n">
+      <c r="Z4" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="AA4" s="23" t="n">
+      <c r="AA4" s="22" t="n">
         <v>21</v>
       </c>
-      <c r="AB4" s="23" t="n">
+      <c r="AB4" s="22" t="n">
         <v>22</v>
       </c>
-      <c r="AC4" s="23" t="n">
+      <c r="AC4" s="22" t="n">
         <v>23</v>
       </c>
-      <c r="AD4" s="23" t="n">
+      <c r="AD4" s="22" t="n">
         <v>24</v>
       </c>
-      <c r="AE4" s="23" t="n">
+      <c r="AE4" s="22" t="n">
         <v>25</v>
       </c>
     </row>
@@ -5183,7 +5215,7 @@
       <c r="L11" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="M11" s="23" t="s">
+      <c r="M11" s="22" t="s">
         <v>262</v>
       </c>
       <c r="N11" s="0" t="s">
@@ -5215,7 +5247,7 @@
       <c r="E12" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="22" t="s">
         <v>261</v>
       </c>
       <c r="N12" s="0" t="s">
@@ -5250,7 +5282,7 @@
       <c r="E13" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="O13" s="23" t="s">
+      <c r="O13" s="22" t="s">
         <v>261</v>
       </c>
       <c r="P13" s="0" t="s">
@@ -5328,7 +5360,7 @@
       <c r="E15" s="34" t="s">
         <v>298</v>
       </c>
-      <c r="Q15" s="23" t="s">
+      <c r="Q15" s="22" t="s">
         <v>299</v>
       </c>
       <c r="R15" s="0" t="s">
@@ -5573,7 +5605,7 @@
       <c r="E22" s="0" t="s">
         <v>321</v>
       </c>
-      <c r="X22" s="23" t="s">
+      <c r="X22" s="22" t="s">
         <v>299</v>
       </c>
       <c r="Y22" s="0" t="s">

</xml_diff>